<commit_message>
Comparison between linear and logistic regression models
</commit_message>
<xml_diff>
--- a/graphs/trends.xlsx
+++ b/graphs/trends.xlsx
@@ -5,16 +5,17 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MSU\Special Topic in CSE Big Data and Data Science\Data_Dawgs\trends\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MSU\Special Topic in CSE Big Data and Data Science\Data_Dawgs\graphs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="28800" windowHeight="17475" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="28800" windowHeight="17475" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="keywords (2)" sheetId="4" r:id="rId1"/>
     <sheet name="keywords" sheetId="1" r:id="rId2"/>
     <sheet name="genres" sheetId="3" r:id="rId3"/>
+    <sheet name="actors" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="87">
   <si>
     <t>gene</t>
   </si>
@@ -227,6 +228,66 @@
   </si>
   <si>
     <t>buyer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leonardo DiCaprio </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kate Winslet </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Julie Andrews </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jim Fitzpatrick </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jennifer Lawrence </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nathan Fillion </t>
+  </si>
+  <si>
+    <t>Philip Seymour Hoffman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ewan McGregor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kohl Sudduth </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vanessa Redgrave </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jude Law </t>
+  </si>
+  <si>
+    <t>Benicio Del Toro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jesse Eisenberg </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corey Burton </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ryan Gosling </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mia Wasikowska </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cher  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edward Norton </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jake Gyllenhaal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sean Penn </t>
   </si>
 </sst>
 </file>
@@ -364,7 +425,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1100,11 +1160,11 @@
         </c:dLbls>
         <c:gapWidth val="269"/>
         <c:overlap val="-20"/>
-        <c:axId val="-2012609568"/>
-        <c:axId val="-2012598688"/>
+        <c:axId val="166712128"/>
+        <c:axId val="166713216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2012609568"/>
+        <c:axId val="166712128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1144,7 +1204,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2012598688"/>
+        <c:crossAx val="166713216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1152,7 +1212,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2012598688"/>
+        <c:axId val="166713216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1199,7 +1259,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2012609568"/>
+        <c:crossAx val="166712128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2034,11 +2094,11 @@
         </c:dLbls>
         <c:gapWidth val="269"/>
         <c:overlap val="-20"/>
-        <c:axId val="-2004089952"/>
-        <c:axId val="-2004088864"/>
+        <c:axId val="166712672"/>
+        <c:axId val="166714304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2004089952"/>
+        <c:axId val="166712672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2078,7 +2138,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2004088864"/>
+        <c:crossAx val="166714304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2086,7 +2146,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2004088864"/>
+        <c:axId val="166714304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2133,7 +2193,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2004089952"/>
+        <c:crossAx val="166712672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2729,11 +2789,11 @@
         </c:dLbls>
         <c:gapWidth val="269"/>
         <c:overlap val="-20"/>
-        <c:axId val="-2004088320"/>
-        <c:axId val="-2004084512"/>
+        <c:axId val="166716480"/>
+        <c:axId val="166461504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2004088320"/>
+        <c:axId val="166716480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2773,7 +2833,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2004084512"/>
+        <c:crossAx val="166461504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2781,7 +2841,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2004084512"/>
+        <c:axId val="166461504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2828,7 +2888,812 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2004088320"/>
+        <c:crossAx val="166716480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg2">
+        <a:lumMod val="50000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="0" u="sng">
+                <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+                <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              </a:rPr>
+              <a:t>A</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="0">
+                <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+                <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              </a:rPr>
+              <a:t>CTORS feature co-efficients</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="0" baseline="0">
+                <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+                <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              </a:rPr>
+              <a:t> in a simple linear regression model|</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" b="0">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="ltUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="accent1"/>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="lt1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="ltUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="accent2"/>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="lt1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="ltUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="accent3"/>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="lt1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="ltUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="accent4"/>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="lt1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="ltUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="accent5"/>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="lt1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="ltUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="accent6"/>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="lt1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="ltUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="lt1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="ltUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="lt1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="ltUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="lt1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="ltUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="lt1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="ltUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="lt1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="ltUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="lt1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="ltUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="lt1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="ltUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="lt1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="14"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="ltUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="lt1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="15"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="ltUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="lt1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="16"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="ltUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="lt1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="17"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="ltUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="lt1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="18"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="ltUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="80000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="lt1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="19"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="ltUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="80000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="lt1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>actors!$A$1:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>Leonardo DiCaprio </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Kate Winslet </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Julie Andrews </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Jim Fitzpatrick </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Jennifer Lawrence </c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Nathan Fillion </c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Philip Seymour Hoffman</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Ewan McGregor </c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Kohl Sudduth </c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Vanessa Redgrave </c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Jude Law </c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Benicio Del Toro</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Jesse Eisenberg </c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Corey Burton </c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Ryan Gosling </c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Mia Wasikowska </c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Cher  </c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Edward Norton </c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Jake Gyllenhaal </c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Sean Penn </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>actors!$B$1:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1.4008071588</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.39322266287</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3316331007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2833395782699999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.25320871281</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2133981782300001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1910752366699999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1632692920900001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.16322292638</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.1406065920999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.13319675562</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1298856072400001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.1275268407000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.1133500757399999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.1132613201499999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.0965482880899999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.086742012</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.0757553412</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.0716734433499999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.0678633745399999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="269"/>
+        <c:overlap val="-20"/>
+        <c:axId val="166648080"/>
+        <c:axId val="166642096"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="166648080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="166642096"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="166642096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="166648080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2996,6 +3861,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="226">
   <cs:axisTitle>
@@ -4069,6 +4974,542 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="226">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="150" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
+          <a:schemeClr val="phClr"/>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="22225">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="35000"/>
+          <a:lumOff val="65000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="25400">
+          <a:schemeClr val="lt1"/>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+            <a:tint val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1500" b="1" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="226">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4694,6 +6135,41 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5289,7 +6765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
@@ -5587,7 +7063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -5750,4 +7226,180 @@
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1">
+        <v>1.4008071588</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2">
+        <v>1.39322266287</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3">
+        <v>1.3316331007</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4">
+        <v>1.2833395782699999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5">
+        <v>1.25320871281</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6">
+        <v>1.2133981782300001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7">
+        <v>1.1910752366699999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8">
+        <v>1.1632692920900001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9">
+        <v>1.16322292638</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10">
+        <v>1.1406065920999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11">
+        <v>1.13319675562</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12">
+        <v>1.1298856072400001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13">
+        <v>1.1275268407000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14">
+        <v>1.1133500757399999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15">
+        <v>1.1132613201499999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16">
+        <v>1.0965482880899999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17">
+        <v>1.086742012</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18">
+        <v>1.0757553412</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19">
+        <v>1.0716734433499999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20">
+        <v>1.0678633745399999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added director coefficients json and trend graph
</commit_message>
<xml_diff>
--- a/graphs/trends.xlsx
+++ b/graphs/trends.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="28800" windowHeight="17475" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="28800" windowHeight="17475" tabRatio="500" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="keywords (2)" sheetId="4" r:id="rId1"/>
     <sheet name="keywords" sheetId="1" r:id="rId2"/>
     <sheet name="genres" sheetId="3" r:id="rId3"/>
     <sheet name="actors" sheetId="6" r:id="rId4"/>
+    <sheet name="directors" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="97">
   <si>
     <t>gene</t>
   </si>
@@ -288,6 +289,36 @@
   </si>
   <si>
     <t xml:space="preserve">Sean Penn </t>
+  </si>
+  <si>
+    <t>Quentin Tarantino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">David Fincher </t>
+  </si>
+  <si>
+    <t>Paul Thomas Anderson</t>
+  </si>
+  <si>
+    <t>Wes Anderson</t>
+  </si>
+  <si>
+    <t>George Lucas</t>
+  </si>
+  <si>
+    <t>The Coen Brothers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Martin Scorsese </t>
+  </si>
+  <si>
+    <t>David Lynch</t>
+  </si>
+  <si>
+    <t>John Lasseter</t>
+  </si>
+  <si>
+    <t>Steven Spielberg</t>
   </si>
 </sst>
 </file>
@@ -1160,11 +1191,11 @@
         </c:dLbls>
         <c:gapWidth val="269"/>
         <c:overlap val="-20"/>
-        <c:axId val="166712128"/>
-        <c:axId val="166713216"/>
+        <c:axId val="2020623648"/>
+        <c:axId val="2020624192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="166712128"/>
+        <c:axId val="2020623648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1204,7 +1235,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166713216"/>
+        <c:crossAx val="2020624192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1212,7 +1243,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="166713216"/>
+        <c:axId val="2020624192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1259,7 +1290,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166712128"/>
+        <c:crossAx val="2020623648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1358,7 +1389,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2094,11 +2124,11 @@
         </c:dLbls>
         <c:gapWidth val="269"/>
         <c:overlap val="-20"/>
-        <c:axId val="166712672"/>
-        <c:axId val="166714304"/>
+        <c:axId val="2020619840"/>
+        <c:axId val="2020610048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="166712672"/>
+        <c:axId val="2020619840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2138,7 +2168,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166714304"/>
+        <c:crossAx val="2020610048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2146,7 +2176,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="166714304"/>
+        <c:axId val="2020610048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2193,7 +2223,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166712672"/>
+        <c:crossAx val="2020619840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2288,7 +2318,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2789,11 +2818,11 @@
         </c:dLbls>
         <c:gapWidth val="269"/>
         <c:overlap val="-20"/>
-        <c:axId val="166716480"/>
-        <c:axId val="166461504"/>
+        <c:axId val="2020612224"/>
+        <c:axId val="2020616576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="166716480"/>
+        <c:axId val="2020612224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2833,7 +2862,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166461504"/>
+        <c:crossAx val="2020616576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2841,7 +2870,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="166461504"/>
+        <c:axId val="2020616576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2888,7 +2917,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166716480"/>
+        <c:crossAx val="2020612224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3594,11 +3623,11 @@
         </c:dLbls>
         <c:gapWidth val="269"/>
         <c:overlap val="-20"/>
-        <c:axId val="166648080"/>
-        <c:axId val="166642096"/>
+        <c:axId val="1985858544"/>
+        <c:axId val="1985860720"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="166648080"/>
+        <c:axId val="1985858544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3638,7 +3667,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166642096"/>
+        <c:crossAx val="1985860720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3646,7 +3675,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="166642096"/>
+        <c:axId val="1985860720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3693,7 +3722,539 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166648080"/>
+        <c:crossAx val="1985858544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg2">
+        <a:lumMod val="50000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="0" u="sng">
+                <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+                <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              </a:rPr>
+              <a:t>H</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="0">
+                <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+                <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              </a:rPr>
+              <a:t>ighest Director co-efficients</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="0" baseline="0">
+                <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+                <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              </a:rPr>
+              <a:t> in a simple linear regression model|</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" b="0">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Test</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="ltUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="accent1"/>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="lt1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="ltUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="accent2"/>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="lt1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="ltUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="accent3"/>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="lt1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="ltUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="accent4"/>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="lt1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="ltUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="accent5"/>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="lt1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="ltUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="accent6"/>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="lt1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="ltUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="lt1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="ltUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="lt1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="ltUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="lt1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:pattFill prst="ltUpDiag">
+                <a:fgClr>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="lt1"/>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>directors!$A$1:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Quentin Tarantino</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>David Fincher </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Paul Thomas Anderson</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Wes Anderson</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>George Lucas</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>The Coen Brothers</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Martin Scorsese </c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>David Lynch</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>John Lasseter</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Steven Spielberg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>directors!$B$1:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.8356352765299999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8134813545099999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.57324059866</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5132949359300001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4932326272000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4732306343299999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4679510711099999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.3418424491600001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.3299095220999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.21359169109</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="269"/>
+        <c:overlap val="-20"/>
+        <c:axId val="123252992"/>
+        <c:axId val="123247008"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="123252992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="123247008"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="123247008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="123252992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3901,6 +4462,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="226">
   <cs:axisTitle>
@@ -5510,6 +6111,542 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="226">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="150" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
+          <a:schemeClr val="phClr"/>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="22225">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="35000"/>
+          <a:lumOff val="65000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="25400">
+          <a:schemeClr val="lt1"/>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+            <a:tint val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1500" b="1" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="226">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6187,6 +7324,41 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -7232,7 +8404,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
+    <sheetView topLeftCell="E2" workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
@@ -7402,4 +8574,191 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F3" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1">
+        <v>1.8356352765299999</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2">
+        <v>1.8134813545099999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3">
+        <v>1.57324059866</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4">
+        <v>1.5132949359300001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5">
+        <v>1.4932326272000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6">
+        <v>1.4732306343299999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7">
+        <v>1.4679510711099999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8">
+        <v>1.3418424491600001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9">
+        <v>1.3299095220999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10">
+        <v>1.21359169109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>